<commit_message>
Start on COCO process
</commit_message>
<xml_diff>
--- a/notebooks/datasets_classes/Grouped_classes.xlsx
+++ b/notebooks/datasets_classes/Grouped_classes.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,22 +8,37 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\taren\GitHub\SquareEyes\notebooks\datasets_classes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{8BCB0599-E5CF-43A5-968C-33EFB3C379E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF0097DB-22FC-4A7C-AAA7-6774A48EE5A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28695" yWindow="2235" windowWidth="29010" windowHeight="28470" activeTab="4"/>
+    <workbookView xWindow="28695" yWindow="2235" windowWidth="15495" windowHeight="28470" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Helper" sheetId="3" r:id="rId1"/>
-    <sheet name="coco_classes" sheetId="1" r:id="rId2"/>
-    <sheet name="obj365_classes" sheetId="2" r:id="rId3"/>
-    <sheet name="OpenImages_classes" sheetId="4" r:id="rId4"/>
-    <sheet name="ImageNet_classes" sheetId="5" r:id="rId5"/>
+    <sheet name="Grouped" sheetId="6" r:id="rId2"/>
+    <sheet name="Codes" sheetId="7" r:id="rId3"/>
+    <sheet name="coco_classes" sheetId="1" r:id="rId4"/>
+    <sheet name="obj365_classes" sheetId="2" r:id="rId5"/>
+    <sheet name="OpenImages_classes" sheetId="4" r:id="rId6"/>
+    <sheet name="ImageNet_classes" sheetId="5" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">ImageNet_classes!$A$1:$G$1001</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">OpenImages_classes!$A$1:$F$602</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">ImageNet_classes!$A$1:$G$1001</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">OpenImages_classes!$A$1:$F$602</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -50,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3886" uniqueCount="3495">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4144" uniqueCount="3512">
   <si>
     <t>person</t>
   </si>
@@ -10535,13 +10550,64 @@
   </si>
   <si>
     <t>Probably can't use</t>
+  </si>
+  <si>
+    <t>Coco</t>
+  </si>
+  <si>
+    <t>Obj365</t>
+  </si>
+  <si>
+    <t>OpenImages</t>
+  </si>
+  <si>
+    <t>ImageNet</t>
+  </si>
+  <si>
+    <t>Square Eyes Code</t>
+  </si>
+  <si>
+    <t>Model Code</t>
+  </si>
+  <si>
+    <t>Dataset</t>
+  </si>
+  <si>
+    <t>Computer Monitor</t>
+  </si>
+  <si>
+    <t>Mobile Device (phone, ipod)</t>
+  </si>
+  <si>
+    <t>Mobile Phone</t>
+  </si>
+  <si>
+    <t>Tablet (ipad, e-reader)</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Screens only</t>
+  </si>
+  <si>
+    <t>Screens + Indicators</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Computer Mouse</t>
+  </si>
+  <si>
+    <t>Computer Keyboard</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -10676,8 +10742,17 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -10857,6 +10932,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -11018,8 +11099,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -11374,11 +11458,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11445,14 +11529,1833 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C81"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBBA4564-078A-4427-8BA8-419A76B666DA}">
+  <dimension ref="B1:AO67"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="V33" sqref="V33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="14" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="60.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="44.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="27" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="34" max="37" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="30.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:41" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>3495</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3496</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3497</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3498</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3495</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>3496</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>3497</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>3498</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>3495</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>3496</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>3497</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>3498</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>3495</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>3496</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>3497</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>3498</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>3495</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>3496</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>3497</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>3498</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>3495</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>3496</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>3497</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>3498</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>3495</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>3496</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>3497</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>3498</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>3495</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>3496</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>3497</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>3498</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>3495</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>3496</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>3497</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>3498</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>3495</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>3496</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>3497</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>3498</v>
+      </c>
+    </row>
+    <row r="2" spans="2:41" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="AK2" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="AL2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AM2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AN2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AO2" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="2:41" x14ac:dyDescent="0.25">
+      <c r="B3" t="str" cm="1">
+        <f t="array" ref="B3">IFERROR(_xlfn._xlws.FILTER(coco_classes!$B:$B,coco_classes!$C:$C=Grouped!B2),"")</f>
+        <v/>
+      </c>
+      <c r="C3" s="3" t="str" cm="1">
+        <f t="array" ref="C3">IFERROR(_xlfn._xlws.FILTER(obj365_classes!$B:$B,obj365_classes!$C:$C=Grouped!C2),"")</f>
+        <v>ComputerBox</v>
+      </c>
+      <c r="D3" s="3" t="str" cm="1">
+        <f t="array" ref="D3">IFERROR(_xlfn._xlws.FILTER(OpenImages_classes!$B:$B,OpenImages_classes!$C:$C=Grouped!D2),"")</f>
+        <v>Computer monitor</v>
+      </c>
+      <c r="E3" s="3" t="str" cm="1">
+        <f t="array" ref="E3:E4">IFERROR(_xlfn._xlws.FILTER(ImageNet_classes!$B:$B,ImageNet_classes!$C:$C=Grouped!E2),"")</f>
+        <v>desktop computer</v>
+      </c>
+      <c r="F3" s="3" t="str" cm="1">
+        <f t="array" ref="F3">IFERROR(_xlfn._xlws.FILTER(coco_classes!$B:$B,coco_classes!$C:$C=Grouped!F2),"")</f>
+        <v>laptop</v>
+      </c>
+      <c r="G3" s="3" t="str" cm="1">
+        <f t="array" ref="G3">IFERROR(_xlfn._xlws.FILTER(obj365_classes!$B:$B,obj365_classes!$C:$C=Grouped!G2),"")</f>
+        <v>Laptop</v>
+      </c>
+      <c r="H3" s="3" t="str" cm="1">
+        <f t="array" ref="H3">IFERROR(_xlfn._xlws.FILTER(OpenImages_classes!$B:$B,OpenImages_classes!$C:$C=Grouped!H2),"")</f>
+        <v>Laptop</v>
+      </c>
+      <c r="I3" s="3" t="str" cm="1">
+        <f t="array" ref="I3:I4">IFERROR(_xlfn._xlws.FILTER(ImageNet_classes!$B:$B,ImageNet_classes!$C:$C=Grouped!I2),"")</f>
+        <v>laptop, laptop computer</v>
+      </c>
+      <c r="J3" s="3" t="str" cm="1">
+        <f t="array" ref="J3">IFERROR(_xlfn._xlws.FILTER(coco_classes!$B:$B,coco_classes!$C:$C=Grouped!J2),"")</f>
+        <v>cellphone</v>
+      </c>
+      <c r="K3" s="3" t="str" cm="1">
+        <f t="array" ref="K3">IFERROR(_xlfn._xlws.FILTER(obj365_classes!$B:$B,obj365_classes!$C:$C=Grouped!K2),"")</f>
+        <v>CellPhone</v>
+      </c>
+      <c r="L3" s="3" t="str" cm="1">
+        <f t="array" ref="L3:L4">IFERROR(_xlfn._xlws.FILTER(OpenImages_classes!$B:$B,OpenImages_classes!$C:$C=Grouped!L2),"")</f>
+        <v>Ipod</v>
+      </c>
+      <c r="M3" s="3" t="str" cm="1">
+        <f t="array" ref="M3:M4">IFERROR(_xlfn._xlws.FILTER(ImageNet_classes!$B:$B,ImageNet_classes!$C:$C=Grouped!M2),"")</f>
+        <v>cellular telephone, cellular phone, cellphone, cell, mobile phone</v>
+      </c>
+      <c r="N3" t="str" cm="1">
+        <f t="array" ref="N3">IFERROR(_xlfn._xlws.FILTER(coco_classes!$B:$B,coco_classes!$C:$C=Grouped!N2),"")</f>
+        <v/>
+      </c>
+      <c r="O3" t="str" cm="1">
+        <f t="array" ref="O3">IFERROR(_xlfn._xlws.FILTER(obj365_classes!$B:$B,obj365_classes!$C:$C=Grouped!O2),"")</f>
+        <v/>
+      </c>
+      <c r="P3" t="str" cm="1">
+        <f t="array" ref="P3">IFERROR(_xlfn._xlws.FILTER(OpenImages_classes!$B:$B,OpenImages_classes!$C:$C=Grouped!P2),"")</f>
+        <v/>
+      </c>
+      <c r="Q3" s="3" t="str" cm="1">
+        <f t="array" ref="Q3">IFERROR(_xlfn._xlws.FILTER(ImageNet_classes!$B:$B,ImageNet_classes!$C:$C=Grouped!Q2),"")</f>
+        <v>hand-held computer, hand-held microcomputer</v>
+      </c>
+      <c r="R3" s="3" t="str" cm="1">
+        <f t="array" ref="R3">IFERROR(_xlfn._xlws.FILTER(coco_classes!$B:$B,coco_classes!$C:$C=Grouped!R2),"")</f>
+        <v>tv</v>
+      </c>
+      <c r="S3" t="str" cm="1">
+        <f t="array" ref="S3">IFERROR(_xlfn._xlws.FILTER(obj365_classes!$B:$B,obj365_classes!$C:$C=Grouped!S2),"")</f>
+        <v/>
+      </c>
+      <c r="T3" s="3" t="str" cm="1">
+        <f t="array" ref="T3">IFERROR(_xlfn._xlws.FILTER(OpenImages_classes!$B:$B,OpenImages_classes!$C:$C=Grouped!T2),"")</f>
+        <v>Television</v>
+      </c>
+      <c r="U3" s="3" t="str" cm="1">
+        <f t="array" ref="U3:U4">IFERROR(_xlfn._xlws.FILTER(ImageNet_classes!$B:$B,ImageNet_classes!$C:$C=Grouped!U2),"")</f>
+        <v>screen, CRT screen</v>
+      </c>
+      <c r="V3" s="3" t="str" cm="1">
+        <f t="array" ref="V3:V5">IFERROR(_xlfn._xlws.FILTER(coco_classes!$B:$B,coco_classes!$C:$C=Grouped!V2),"")</f>
+        <v>mouse</v>
+      </c>
+      <c r="W3" s="3" t="str" cm="1">
+        <f t="array" ref="W3:W5">IFERROR(_xlfn._xlws.FILTER(obj365_classes!$B:$B,obj365_classes!$C:$C=Grouped!W2),"")</f>
+        <v>Keyboard</v>
+      </c>
+      <c r="X3" s="3" t="str" cm="1">
+        <f t="array" ref="X3:X5">IFERROR(_xlfn._xlws.FILTER(OpenImages_classes!$B:$B,OpenImages_classes!$C:$C=Grouped!X2),"")</f>
+        <v>Computer keyboard</v>
+      </c>
+      <c r="Y3" s="3" t="str" cm="1">
+        <f t="array" ref="Y3:Y4">IFERROR(_xlfn._xlws.FILTER(ImageNet_classes!$B:$B,ImageNet_classes!$C:$C=Grouped!Y2),"")</f>
+        <v>computer keyboard, keypad</v>
+      </c>
+      <c r="Z3" t="str" cm="1">
+        <f t="array" ref="Z3">IFERROR(_xlfn._xlws.FILTER(coco_classes!$B:$B,coco_classes!$C:$C=Grouped!Z2),"")</f>
+        <v>book</v>
+      </c>
+      <c r="AA3" t="str" cm="1">
+        <f t="array" ref="AA3">IFERROR(_xlfn._xlws.FILTER(obj365_classes!$B:$B,obj365_classes!$C:$C=Grouped!AA2),"")</f>
+        <v>Book</v>
+      </c>
+      <c r="AB3" t="str" cm="1">
+        <f t="array" ref="AB3">IFERROR(_xlfn._xlws.FILTER(OpenImages_classes!$B:$B,OpenImages_classes!$C:$C=Grouped!AB2),"")</f>
+        <v>Book</v>
+      </c>
+      <c r="AC3" t="str" cm="1">
+        <f t="array" ref="AC3">IFERROR(_xlfn._xlws.FILTER(ImageNet_classes!$B:$B,ImageNet_classes!$C:$C=Grouped!AC2),"")</f>
+        <v/>
+      </c>
+      <c r="AD3" t="str" cm="1">
+        <f t="array" ref="AD3">IFERROR(_xlfn._xlws.FILTER(coco_classes!$B:$B,coco_classes!$C:$C=Grouped!AD2),"")</f>
+        <v/>
+      </c>
+      <c r="AE3" t="str" cm="1">
+        <f t="array" ref="AE3">IFERROR(_xlfn._xlws.FILTER(obj365_classes!$B:$B,obj365_classes!$C:$C=Grouped!AE2),"")</f>
+        <v>Notepaper</v>
+      </c>
+      <c r="AF3" t="str" cm="1">
+        <f t="array" ref="AF3">IFERROR(_xlfn._xlws.FILTER(OpenImages_classes!$B:$B,OpenImages_classes!$C:$C=Grouped!AF2),"")</f>
+        <v/>
+      </c>
+      <c r="AG3" t="str" cm="1">
+        <f t="array" ref="AG3">IFERROR(_xlfn._xlws.FILTER(ImageNet_classes!$B:$B,ImageNet_classes!$C:$C=Grouped!AG2),"")</f>
+        <v/>
+      </c>
+      <c r="AH3" t="str" cm="1">
+        <f t="array" ref="AH3">IFERROR(_xlfn._xlws.FILTER(coco_classes!$B:$B,coco_classes!$C:$C=Grouped!AH2),"")</f>
+        <v/>
+      </c>
+      <c r="AI3" t="str" cm="1">
+        <f t="array" ref="AI3">IFERROR(_xlfn._xlws.FILTER(obj365_classes!$B:$B,obj365_classes!$C:$C=Grouped!AI2),"")</f>
+        <v>Pen/Pencil</v>
+      </c>
+      <c r="AJ3" t="str" cm="1">
+        <f t="array" ref="AJ3">IFERROR(_xlfn._xlws.FILTER(OpenImages_classes!$B:$B,OpenImages_classes!$C:$C=Grouped!AJ2),"")</f>
+        <v>Pen</v>
+      </c>
+      <c r="AK3" t="str" cm="1">
+        <f t="array" ref="AK3">IFERROR(_xlfn._xlws.FILTER(ImageNet_classes!$B:$B,ImageNet_classes!$C:$C=Grouped!AK2),"")</f>
+        <v/>
+      </c>
+      <c r="AL3" t="str" cm="1">
+        <f t="array" ref="AL3:AL17">IFERROR(_xlfn._xlws.FILTER(coco_classes!$B:$B,coco_classes!$C:$C=Grouped!AL2),"")</f>
+        <v>cup</v>
+      </c>
+      <c r="AM3" t="str" cm="1">
+        <f t="array" ref="AM3:AM67">IFERROR(_xlfn._xlws.FILTER(obj365_classes!$B:$B,obj365_classes!$C:$C=Grouped!AM2),"")</f>
+        <v>Cup</v>
+      </c>
+      <c r="AN3" t="str" cm="1">
+        <f t="array" ref="AN3:AN60">IFERROR(_xlfn._xlws.FILTER(OpenImages_classes!$B:$B,OpenImages_classes!$C:$C=Grouped!AN2),"")</f>
+        <v>Apple</v>
+      </c>
+      <c r="AO3" t="str" cm="1">
+        <f t="array" ref="AO3:AO46">IFERROR(_xlfn._xlws.FILTER(ImageNet_classes!$B:$B,ImageNet_classes!$C:$C=Grouped!AO2),"")</f>
+        <v>plate</v>
+      </c>
+    </row>
+    <row r="4" spans="2:41" x14ac:dyDescent="0.25">
+      <c r="E4" s="3" t="str">
+        <v>monitor</v>
+      </c>
+      <c r="I4" s="3" t="str">
+        <v>notebook, notebook computer</v>
+      </c>
+      <c r="L4" s="3" t="str">
+        <v>Mobile phone</v>
+      </c>
+      <c r="M4" s="3" t="str">
+        <v>iPod</v>
+      </c>
+      <c r="U4" s="3" t="str">
+        <v>television, television system</v>
+      </c>
+      <c r="V4" s="3" t="str">
+        <v>remote</v>
+      </c>
+      <c r="W4" s="3" t="str">
+        <v>Mouse</v>
+      </c>
+      <c r="X4" s="3" t="str">
+        <v>Computer mouse</v>
+      </c>
+      <c r="Y4" s="3" t="str">
+        <v>mouse, computer mouse</v>
+      </c>
+      <c r="AL4" t="str">
+        <v>fork</v>
+      </c>
+      <c r="AM4" t="str">
+        <v>Plate</v>
+      </c>
+      <c r="AN4" t="str">
+        <v>Bagel</v>
+      </c>
+      <c r="AO4" t="str">
+        <v>guacamole</v>
+      </c>
+    </row>
+    <row r="5" spans="2:41" x14ac:dyDescent="0.25">
+      <c r="V5" s="3" t="str">
+        <v>keyboard</v>
+      </c>
+      <c r="W5" s="3" t="str">
+        <v>Remote</v>
+      </c>
+      <c r="X5" s="3" t="str">
+        <v>Remote control</v>
+      </c>
+      <c r="Y5" s="3"/>
+      <c r="AL5" t="str">
+        <v>knife</v>
+      </c>
+      <c r="AM5" t="str">
+        <v>Bread</v>
+      </c>
+      <c r="AN5" t="str">
+        <v>Baked goods</v>
+      </c>
+      <c r="AO5" t="str">
+        <v>hot pot, hotpot</v>
+      </c>
+    </row>
+    <row r="6" spans="2:41" x14ac:dyDescent="0.25">
+      <c r="AL6" t="str">
+        <v>spoon</v>
+      </c>
+      <c r="AM6" t="str">
+        <v>Apple</v>
+      </c>
+      <c r="AN6" t="str">
+        <v>Banana</v>
+      </c>
+      <c r="AO6" t="str">
+        <v>trifle</v>
+      </c>
+    </row>
+    <row r="7" spans="2:41" x14ac:dyDescent="0.25">
+      <c r="AL7" t="str">
+        <v>bowl</v>
+      </c>
+      <c r="AM7" t="str">
+        <v>Knife</v>
+      </c>
+      <c r="AN7" t="str">
+        <v>Bell pepper</v>
+      </c>
+      <c r="AO7" t="str">
+        <v>ice cream, icecream</v>
+      </c>
+    </row>
+    <row r="8" spans="2:41" x14ac:dyDescent="0.25">
+      <c r="AL8" t="str">
+        <v>banana</v>
+      </c>
+      <c r="AM8" t="str">
+        <v>Fork</v>
+      </c>
+      <c r="AN8" t="str">
+        <v>Bowl</v>
+      </c>
+      <c r="AO8" t="str">
+        <v>ice lolly, lolly, lollipop, popsicle</v>
+      </c>
+    </row>
+    <row r="9" spans="2:41" x14ac:dyDescent="0.25">
+      <c r="AL9" t="str">
+        <v>apple</v>
+      </c>
+      <c r="AM9" t="str">
+        <v>Spoon</v>
+      </c>
+      <c r="AN9" t="str">
+        <v>Bread</v>
+      </c>
+      <c r="AO9" t="str">
+        <v>French loaf</v>
+      </c>
+    </row>
+    <row r="10" spans="2:41" x14ac:dyDescent="0.25">
+      <c r="AL10" t="str">
+        <v>sandwich</v>
+      </c>
+      <c r="AM10" t="str">
+        <v>Cake</v>
+      </c>
+      <c r="AN10" t="str">
+        <v>Broccoli</v>
+      </c>
+      <c r="AO10" t="str">
+        <v>bagel, beigel</v>
+      </c>
+    </row>
+    <row r="11" spans="2:41" x14ac:dyDescent="0.25">
+      <c r="AL11" t="str">
+        <v>orange</v>
+      </c>
+      <c r="AM11" t="str">
+        <v>Tomato</v>
+      </c>
+      <c r="AN11" t="str">
+        <v>Burrito</v>
+      </c>
+      <c r="AO11" t="str">
+        <v>pretzel</v>
+      </c>
+    </row>
+    <row r="12" spans="2:41" x14ac:dyDescent="0.25">
+      <c r="AL12" t="str">
+        <v>broccoli</v>
+      </c>
+      <c r="AM12" t="str">
+        <v>GreenVegetables</v>
+      </c>
+      <c r="AN12" t="str">
+        <v>Cabbage</v>
+      </c>
+      <c r="AO12" t="str">
+        <v>cheeseburger</v>
+      </c>
+    </row>
+    <row r="13" spans="2:41" x14ac:dyDescent="0.25">
+      <c r="AL13" t="str">
+        <v>carrot</v>
+      </c>
+      <c r="AM13" t="str">
+        <v>Banana</v>
+      </c>
+      <c r="AN13" t="str">
+        <v>Cake</v>
+      </c>
+      <c r="AO13" t="str">
+        <v>hotdog, hot dog, red hot</v>
+      </c>
+    </row>
+    <row r="14" spans="2:41" x14ac:dyDescent="0.25">
+      <c r="AL14" t="str">
+        <v>hotdog</v>
+      </c>
+      <c r="AM14" t="str">
+        <v>Dessert</v>
+      </c>
+      <c r="AN14" t="str">
+        <v>Candy</v>
+      </c>
+      <c r="AO14" t="str">
+        <v>mashed potato</v>
+      </c>
+    </row>
+    <row r="15" spans="2:41" x14ac:dyDescent="0.25">
+      <c r="AL15" t="str">
+        <v>pizza</v>
+      </c>
+      <c r="AM15" t="str">
+        <v>Broccoli</v>
+      </c>
+      <c r="AN15" t="str">
+        <v>Cantaloupe</v>
+      </c>
+      <c r="AO15" t="str">
+        <v>head cabbage</v>
+      </c>
+    </row>
+    <row r="16" spans="2:41" x14ac:dyDescent="0.25">
+      <c r="AL16" t="str">
+        <v>donut</v>
+      </c>
+      <c r="AM16" t="str">
+        <v>Pizza</v>
+      </c>
+      <c r="AN16" t="str">
+        <v>Carrot</v>
+      </c>
+      <c r="AO16" t="str">
+        <v>broccoli</v>
+      </c>
+    </row>
+    <row r="17" spans="38:41" x14ac:dyDescent="0.25">
+      <c r="AL17" t="str">
+        <v>cake</v>
+      </c>
+      <c r="AM17" t="str">
+        <v>Donut</v>
+      </c>
+      <c r="AN17" t="str">
+        <v>Cheese</v>
+      </c>
+      <c r="AO17" t="str">
+        <v>cauliflower</v>
+      </c>
+    </row>
+    <row r="18" spans="38:41" x14ac:dyDescent="0.25">
+      <c r="AM18" t="str">
+        <v>Carrot</v>
+      </c>
+      <c r="AN18" t="str">
+        <v>Coconut</v>
+      </c>
+      <c r="AO18" t="str">
+        <v>zucchini, courgette</v>
+      </c>
+    </row>
+    <row r="19" spans="38:41" x14ac:dyDescent="0.25">
+      <c r="AM19" t="str">
+        <v>Strawberry</v>
+      </c>
+      <c r="AN19" t="str">
+        <v>Coffee (drink)</v>
+      </c>
+      <c r="AO19" t="str">
+        <v>spaghetti squash</v>
+      </c>
+    </row>
+    <row r="20" spans="38:41" x14ac:dyDescent="0.25">
+      <c r="AM20" t="str">
+        <v>Pepper</v>
+      </c>
+      <c r="AN20" t="str">
+        <v>Cookie</v>
+      </c>
+      <c r="AO20" t="str">
+        <v>acorn squash</v>
+      </c>
+    </row>
+    <row r="21" spans="38:41" x14ac:dyDescent="0.25">
+      <c r="AM21" t="str">
+        <v>Pie</v>
+      </c>
+      <c r="AN21" t="str">
+        <v>Croissant</v>
+      </c>
+      <c r="AO21" t="str">
+        <v>butternut squash</v>
+      </c>
+    </row>
+    <row r="22" spans="38:41" x14ac:dyDescent="0.25">
+      <c r="AM22" t="str">
+        <v>Cookies</v>
+      </c>
+      <c r="AN22" t="str">
+        <v>Cucumber</v>
+      </c>
+      <c r="AO22" t="str">
+        <v>cucumber, cuke</v>
+      </c>
+    </row>
+    <row r="23" spans="38:41" x14ac:dyDescent="0.25">
+      <c r="AM23" t="str">
+        <v>Grape</v>
+      </c>
+      <c r="AN23" t="str">
+        <v>Dairy Product</v>
+      </c>
+      <c r="AO23" t="str">
+        <v>artichoke, globe artichoke</v>
+      </c>
+    </row>
+    <row r="24" spans="38:41" x14ac:dyDescent="0.25">
+      <c r="AM24" t="str">
+        <v>Potato</v>
+      </c>
+      <c r="AN24" t="str">
+        <v>Dessert</v>
+      </c>
+      <c r="AO24" t="str">
+        <v>bell pepper</v>
+      </c>
+    </row>
+    <row r="25" spans="38:41" x14ac:dyDescent="0.25">
+      <c r="AM25" t="str">
+        <v>Sausage</v>
+      </c>
+      <c r="AN25" t="str">
+        <v>Drink</v>
+      </c>
+      <c r="AO25" t="str">
+        <v>cardoon</v>
+      </c>
+    </row>
+    <row r="26" spans="38:41" x14ac:dyDescent="0.25">
+      <c r="AM26" t="str">
+        <v>Egg</v>
+      </c>
+      <c r="AN26" t="str">
+        <v>Egg</v>
+      </c>
+      <c r="AO26" t="str">
+        <v>mushroom</v>
+      </c>
+    </row>
+    <row r="27" spans="38:41" x14ac:dyDescent="0.25">
+      <c r="AM27" t="str">
+        <v>Candy</v>
+      </c>
+      <c r="AN27" t="str">
+        <v>Fast food</v>
+      </c>
+      <c r="AO27" t="str">
+        <v>Granny Smith</v>
+      </c>
+    </row>
+    <row r="28" spans="38:41" x14ac:dyDescent="0.25">
+      <c r="AM28" t="str">
+        <v>Cucumber</v>
+      </c>
+      <c r="AN28" t="str">
+        <v>Food</v>
+      </c>
+      <c r="AO28" t="str">
+        <v>strawberry</v>
+      </c>
+    </row>
+    <row r="29" spans="38:41" x14ac:dyDescent="0.25">
+      <c r="AM29" t="str">
+        <v>Pear</v>
+      </c>
+      <c r="AN29" t="str">
+        <v>Fork</v>
+      </c>
+      <c r="AO29" t="str">
+        <v>orange</v>
+      </c>
+    </row>
+    <row r="30" spans="38:41" x14ac:dyDescent="0.25">
+      <c r="AM30" t="str">
+        <v>Hamburger</v>
+      </c>
+      <c r="AN30" t="str">
+        <v>French fries</v>
+      </c>
+      <c r="AO30" t="str">
+        <v>lemon</v>
+      </c>
+    </row>
+    <row r="31" spans="38:41" x14ac:dyDescent="0.25">
+      <c r="AM31" t="str">
+        <v>Onion</v>
+      </c>
+      <c r="AN31" t="str">
+        <v>Grape</v>
+      </c>
+      <c r="AO31" t="str">
+        <v>fig</v>
+      </c>
+    </row>
+    <row r="32" spans="38:41" x14ac:dyDescent="0.25">
+      <c r="AM32" t="str">
+        <v>Greenbeans</v>
+      </c>
+      <c r="AN32" t="str">
+        <v>Grapefruit</v>
+      </c>
+      <c r="AO32" t="str">
+        <v>pineapple, ananas</v>
+      </c>
+    </row>
+    <row r="33" spans="39:41" x14ac:dyDescent="0.25">
+      <c r="AM33" t="str">
+        <v>Watermelon</v>
+      </c>
+      <c r="AN33" t="str">
+        <v>Guacamole</v>
+      </c>
+      <c r="AO33" t="str">
+        <v>banana</v>
+      </c>
+    </row>
+    <row r="34" spans="39:41" x14ac:dyDescent="0.25">
+      <c r="AM34" t="str">
+        <v>FrenchFries</v>
+      </c>
+      <c r="AN34" t="str">
+        <v>Hamburger</v>
+      </c>
+      <c r="AO34" t="str">
+        <v>jackfruit, jak, jack</v>
+      </c>
+    </row>
+    <row r="35" spans="39:41" x14ac:dyDescent="0.25">
+      <c r="AM35" t="str">
+        <v>Hotdog</v>
+      </c>
+      <c r="AN35" t="str">
+        <v>Hot dog</v>
+      </c>
+      <c r="AO35" t="str">
+        <v>custard apple</v>
+      </c>
+    </row>
+    <row r="36" spans="39:41" x14ac:dyDescent="0.25">
+      <c r="AM36" t="str">
+        <v>Peach</v>
+      </c>
+      <c r="AN36" t="str">
+        <v>Ice cream</v>
+      </c>
+      <c r="AO36" t="str">
+        <v>pomegranate</v>
+      </c>
+    </row>
+    <row r="37" spans="39:41" x14ac:dyDescent="0.25">
+      <c r="AM37" t="str">
+        <v>Rice</v>
+      </c>
+      <c r="AN37" t="str">
+        <v>Juice</v>
+      </c>
+      <c r="AO37" t="str">
+        <v>hay</v>
+      </c>
+    </row>
+    <row r="38" spans="39:41" x14ac:dyDescent="0.25">
+      <c r="AM38" t="str">
+        <v>Pineapple</v>
+      </c>
+      <c r="AN38" t="str">
+        <v>Knife</v>
+      </c>
+      <c r="AO38" t="str">
+        <v>carbonara</v>
+      </c>
+    </row>
+    <row r="39" spans="39:41" x14ac:dyDescent="0.25">
+      <c r="AM39" t="str">
+        <v>Mango</v>
+      </c>
+      <c r="AN39" t="str">
+        <v>Mango</v>
+      </c>
+      <c r="AO39" t="str">
+        <v>chocolate sauce, chocolate syrup</v>
+      </c>
+    </row>
+    <row r="40" spans="39:41" x14ac:dyDescent="0.25">
+      <c r="AM40" t="str">
+        <v>Corn</v>
+      </c>
+      <c r="AN40" t="str">
+        <v>Muffin</v>
+      </c>
+      <c r="AO40" t="str">
+        <v>dough</v>
+      </c>
+    </row>
+    <row r="41" spans="39:41" x14ac:dyDescent="0.25">
+      <c r="AM41" t="str">
+        <v>Lettuce</v>
+      </c>
+      <c r="AN41" t="str">
+        <v>Mushroom</v>
+      </c>
+      <c r="AO41" t="str">
+        <v>meat loaf, meatloaf</v>
+      </c>
+    </row>
+    <row r="42" spans="39:41" x14ac:dyDescent="0.25">
+      <c r="AM42" t="str">
+        <v>Garlic</v>
+      </c>
+      <c r="AN42" t="str">
+        <v>Pasta</v>
+      </c>
+      <c r="AO42" t="str">
+        <v>pizza, pizza pie</v>
+      </c>
+    </row>
+    <row r="43" spans="39:41" x14ac:dyDescent="0.25">
+      <c r="AM43" t="str">
+        <v>GreenOnion</v>
+      </c>
+      <c r="AN43" t="str">
+        <v>Pastry</v>
+      </c>
+      <c r="AO43" t="str">
+        <v>potpie</v>
+      </c>
+    </row>
+    <row r="44" spans="39:41" x14ac:dyDescent="0.25">
+      <c r="AM44" t="str">
+        <v>Sandwich</v>
+      </c>
+      <c r="AN44" t="str">
+        <v>Peach</v>
+      </c>
+      <c r="AO44" t="str">
+        <v>burrito</v>
+      </c>
+    </row>
+    <row r="45" spans="39:41" x14ac:dyDescent="0.25">
+      <c r="AM45" t="str">
+        <v>Nuts</v>
+      </c>
+      <c r="AN45" t="str">
+        <v>Pear</v>
+      </c>
+      <c r="AO45" t="str">
+        <v>cup</v>
+      </c>
+    </row>
+    <row r="46" spans="39:41" x14ac:dyDescent="0.25">
+      <c r="AM46" t="str">
+        <v>Plum</v>
+      </c>
+      <c r="AN46" t="str">
+        <v>Pineapple</v>
+      </c>
+      <c r="AO46" t="str">
+        <v>corn</v>
+      </c>
+    </row>
+    <row r="47" spans="39:41" x14ac:dyDescent="0.25">
+      <c r="AM47" t="str">
+        <v>Kiwifruit</v>
+      </c>
+      <c r="AN47" t="str">
+        <v>Pizza</v>
+      </c>
+    </row>
+    <row r="48" spans="39:41" x14ac:dyDescent="0.25">
+      <c r="AM48" t="str">
+        <v>Shrimp</v>
+      </c>
+      <c r="AN48" t="str">
+        <v>Plate</v>
+      </c>
+    </row>
+    <row r="49" spans="39:40" x14ac:dyDescent="0.25">
+      <c r="AM49" t="str">
+        <v>Sushi</v>
+      </c>
+      <c r="AN49" t="str">
+        <v>Popcorn</v>
+      </c>
+    </row>
+    <row r="50" spans="39:40" x14ac:dyDescent="0.25">
+      <c r="AM50" t="str">
+        <v>Cheese</v>
+      </c>
+      <c r="AN50" t="str">
+        <v>Potato</v>
+      </c>
+    </row>
+    <row r="51" spans="39:40" x14ac:dyDescent="0.25">
+      <c r="AM51" t="str">
+        <v>Cherry</v>
+      </c>
+      <c r="AN51" t="str">
+        <v>Pretzel</v>
+      </c>
+    </row>
+    <row r="52" spans="39:40" x14ac:dyDescent="0.25">
+      <c r="AM52" t="str">
+        <v>Pasta</v>
+      </c>
+      <c r="AN52" t="str">
+        <v>Radish</v>
+      </c>
+    </row>
+    <row r="53" spans="39:40" x14ac:dyDescent="0.25">
+      <c r="AM53" t="str">
+        <v>Avocado</v>
+      </c>
+      <c r="AN53" t="str">
+        <v>Sandwich</v>
+      </c>
+    </row>
+    <row r="54" spans="39:40" x14ac:dyDescent="0.25">
+      <c r="AM54" t="str">
+        <v>Mushroom</v>
+      </c>
+      <c r="AN54" t="str">
+        <v>Shrimp</v>
+      </c>
+    </row>
+    <row r="55" spans="39:40" x14ac:dyDescent="0.25">
+      <c r="AM55" t="str">
+        <v>Eggplant</v>
+      </c>
+      <c r="AN55" t="str">
+        <v>Spoon</v>
+      </c>
+    </row>
+    <row r="56" spans="39:40" x14ac:dyDescent="0.25">
+      <c r="AM56" t="str">
+        <v>Coconut</v>
+      </c>
+      <c r="AN56" t="str">
+        <v>Strawberry</v>
+      </c>
+    </row>
+    <row r="57" spans="39:40" x14ac:dyDescent="0.25">
+      <c r="AM57" t="str">
+        <v>Chips</v>
+      </c>
+      <c r="AN57" t="str">
+        <v>Sushi</v>
+      </c>
+    </row>
+    <row r="58" spans="39:40" x14ac:dyDescent="0.25">
+      <c r="AM58" t="str">
+        <v>Steak</v>
+      </c>
+      <c r="AN58" t="str">
+        <v>Tomato</v>
+      </c>
+    </row>
+    <row r="59" spans="39:40" x14ac:dyDescent="0.25">
+      <c r="AM59" t="str">
+        <v>Meatball</v>
+      </c>
+      <c r="AN59" t="str">
+        <v>Watermelon</v>
+      </c>
+    </row>
+    <row r="60" spans="39:40" x14ac:dyDescent="0.25">
+      <c r="AM60" t="str">
+        <v>Papaya</v>
+      </c>
+      <c r="AN60" t="str">
+        <v>Winter melon</v>
+      </c>
+    </row>
+    <row r="61" spans="39:40" x14ac:dyDescent="0.25">
+      <c r="AM61" t="str">
+        <v>Eggtart</v>
+      </c>
+    </row>
+    <row r="62" spans="39:40" x14ac:dyDescent="0.25">
+      <c r="AM62" t="str">
+        <v>Grapefruit</v>
+      </c>
+    </row>
+    <row r="63" spans="39:40" x14ac:dyDescent="0.25">
+      <c r="AM63" t="str">
+        <v>Radish</v>
+      </c>
+    </row>
+    <row r="64" spans="39:40" x14ac:dyDescent="0.25">
+      <c r="AM64" t="str">
+        <v>SpringRolls</v>
+      </c>
+    </row>
+    <row r="65" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM65" t="str">
+        <v>RedCabbage</v>
+      </c>
+    </row>
+    <row r="66" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM66" t="str">
+        <v>Asparagus</v>
+      </c>
+    </row>
+    <row r="67" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM67" t="str">
+        <v>Dumpling</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDFB5A65-B7A8-4EF3-8DCA-3C484E690B5E}">
+  <dimension ref="A1:F32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="54.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>3506</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>3499</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3500</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3501</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3507</v>
+      </c>
+      <c r="B2" t="s">
+        <v>454</v>
+      </c>
+      <c r="C2" t="s">
+        <v>454</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3496</v>
+      </c>
+      <c r="E2">
+        <v>159</v>
+      </c>
+      <c r="F2" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3507</v>
+      </c>
+      <c r="B3" t="s">
+        <v>454</v>
+      </c>
+      <c r="C3" t="s">
+        <v>454</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3498</v>
+      </c>
+      <c r="E3" t="s">
+        <v>2554</v>
+      </c>
+      <c r="F3" t="s">
+        <v>2555</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3507</v>
+      </c>
+      <c r="B4" t="s">
+        <v>454</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3502</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3497</v>
+      </c>
+      <c r="E4" t="s">
+        <v>672</v>
+      </c>
+      <c r="F4" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3507</v>
+      </c>
+      <c r="B5" t="s">
+        <v>454</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3502</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3498</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2828</v>
+      </c>
+      <c r="F5" t="s">
+        <v>2829</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3507</v>
+      </c>
+      <c r="B6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" t="s">
+        <v>85</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3495</v>
+      </c>
+      <c r="E6">
+        <v>63</v>
+      </c>
+      <c r="F6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>3507</v>
+      </c>
+      <c r="B7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D7" t="s">
+        <v>3496</v>
+      </c>
+      <c r="E7">
+        <v>73</v>
+      </c>
+      <c r="F7" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>3507</v>
+      </c>
+      <c r="B8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C8" t="s">
+        <v>85</v>
+      </c>
+      <c r="D8" t="s">
+        <v>3497</v>
+      </c>
+      <c r="E8" t="s">
+        <v>982</v>
+      </c>
+      <c r="F8" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>3507</v>
+      </c>
+      <c r="B9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D9" t="s">
+        <v>3498</v>
+      </c>
+      <c r="E9" t="s">
+        <v>2740</v>
+      </c>
+      <c r="F9" t="s">
+        <v>2741</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>3507</v>
+      </c>
+      <c r="B10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C10" t="s">
+        <v>85</v>
+      </c>
+      <c r="D10" t="s">
+        <v>3498</v>
+      </c>
+      <c r="E10" t="s">
+        <v>2862</v>
+      </c>
+      <c r="F10" t="s">
+        <v>2863</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>3507</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3503</v>
+      </c>
+      <c r="C11" t="s">
+        <v>3504</v>
+      </c>
+      <c r="D11" t="s">
+        <v>3495</v>
+      </c>
+      <c r="E11">
+        <v>67</v>
+      </c>
+      <c r="F11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>3507</v>
+      </c>
+      <c r="B12" t="s">
+        <v>3503</v>
+      </c>
+      <c r="C12" t="s">
+        <v>3504</v>
+      </c>
+      <c r="D12" t="s">
+        <v>3496</v>
+      </c>
+      <c r="E12">
+        <v>61</v>
+      </c>
+      <c r="F12" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>3507</v>
+      </c>
+      <c r="B13" t="s">
+        <v>3503</v>
+      </c>
+      <c r="C13" t="s">
+        <v>3504</v>
+      </c>
+      <c r="D13" t="s">
+        <v>3497</v>
+      </c>
+      <c r="E13" t="s">
+        <v>1045</v>
+      </c>
+      <c r="F13" t="s">
+        <v>1046</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>3507</v>
+      </c>
+      <c r="B14" t="s">
+        <v>3503</v>
+      </c>
+      <c r="C14" t="s">
+        <v>3504</v>
+      </c>
+      <c r="D14" t="s">
+        <v>3498</v>
+      </c>
+      <c r="E14" t="s">
+        <v>2475</v>
+      </c>
+      <c r="F14" t="s">
+        <v>2476</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>3507</v>
+      </c>
+      <c r="B15" t="s">
+        <v>3503</v>
+      </c>
+      <c r="C15" t="s">
+        <v>2711</v>
+      </c>
+      <c r="D15" t="s">
+        <v>3497</v>
+      </c>
+      <c r="E15" t="s">
+        <v>938</v>
+      </c>
+      <c r="F15" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>3507</v>
+      </c>
+      <c r="B16" t="s">
+        <v>3503</v>
+      </c>
+      <c r="C16" t="s">
+        <v>2711</v>
+      </c>
+      <c r="D16" t="s">
+        <v>3498</v>
+      </c>
+      <c r="E16" t="s">
+        <v>2710</v>
+      </c>
+      <c r="F16" t="s">
+        <v>2711</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>3507</v>
+      </c>
+      <c r="B17" t="s">
+        <v>3505</v>
+      </c>
+      <c r="C17" t="s">
+        <v>330</v>
+      </c>
+      <c r="D17" t="s">
+        <v>3498</v>
+      </c>
+      <c r="E17" t="s">
+        <v>2680</v>
+      </c>
+      <c r="F17" t="s">
+        <v>2681</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>3507</v>
+      </c>
+      <c r="B18" t="s">
+        <v>84</v>
+      </c>
+      <c r="C18" t="s">
+        <v>84</v>
+      </c>
+      <c r="D18" t="s">
+        <v>3495</v>
+      </c>
+      <c r="E18">
+        <v>62</v>
+      </c>
+      <c r="F18" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>3507</v>
+      </c>
+      <c r="B19" t="s">
+        <v>84</v>
+      </c>
+      <c r="C19" t="s">
+        <v>84</v>
+      </c>
+      <c r="D19" t="s">
+        <v>3497</v>
+      </c>
+      <c r="E19" t="s">
+        <v>1375</v>
+      </c>
+      <c r="F19" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>3507</v>
+      </c>
+      <c r="B20" t="s">
+        <v>84</v>
+      </c>
+      <c r="C20" t="s">
+        <v>84</v>
+      </c>
+      <c r="D20" t="s">
+        <v>3498</v>
+      </c>
+      <c r="E20" t="s">
+        <v>3202</v>
+      </c>
+      <c r="F20" t="s">
+        <v>3203</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>3507</v>
+      </c>
+      <c r="B21" t="s">
+        <v>84</v>
+      </c>
+      <c r="C21" t="s">
+        <v>84</v>
+      </c>
+      <c r="D21" t="s">
+        <v>3498</v>
+      </c>
+      <c r="E21" t="s">
+        <v>3064</v>
+      </c>
+      <c r="F21" t="s">
+        <v>3065</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>3508</v>
+      </c>
+      <c r="B22" t="s">
+        <v>3509</v>
+      </c>
+      <c r="C22" t="s">
+        <v>3510</v>
+      </c>
+      <c r="D22" t="s">
+        <v>3495</v>
+      </c>
+      <c r="E22">
+        <v>64</v>
+      </c>
+      <c r="F22" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>3508</v>
+      </c>
+      <c r="B23" t="s">
+        <v>3509</v>
+      </c>
+      <c r="C23" t="s">
+        <v>3510</v>
+      </c>
+      <c r="D23" t="s">
+        <v>3496</v>
+      </c>
+      <c r="E23">
+        <v>115</v>
+      </c>
+      <c r="F23" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>3508</v>
+      </c>
+      <c r="B24" t="s">
+        <v>3509</v>
+      </c>
+      <c r="C24" t="s">
+        <v>3510</v>
+      </c>
+      <c r="D24" t="s">
+        <v>3497</v>
+      </c>
+      <c r="E24" t="s">
+        <v>674</v>
+      </c>
+      <c r="F24" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>3508</v>
+      </c>
+      <c r="B25" t="s">
+        <v>3509</v>
+      </c>
+      <c r="C25" t="s">
+        <v>3510</v>
+      </c>
+      <c r="D25" t="s">
+        <v>3498</v>
+      </c>
+      <c r="E25" t="s">
+        <v>2846</v>
+      </c>
+      <c r="F25" t="s">
+        <v>2847</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>3508</v>
+      </c>
+      <c r="B26" t="s">
+        <v>3509</v>
+      </c>
+      <c r="C26" t="s">
+        <v>3511</v>
+      </c>
+      <c r="D26" t="s">
+        <v>3495</v>
+      </c>
+      <c r="E26">
+        <v>66</v>
+      </c>
+      <c r="F26" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>3508</v>
+      </c>
+      <c r="B27" t="s">
+        <v>3509</v>
+      </c>
+      <c r="C27" t="s">
+        <v>3511</v>
+      </c>
+      <c r="D27" t="s">
+        <v>3496</v>
+      </c>
+      <c r="E27">
+        <v>106</v>
+      </c>
+      <c r="F27" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>3508</v>
+      </c>
+      <c r="B28" t="s">
+        <v>3509</v>
+      </c>
+      <c r="C28" t="s">
+        <v>3511</v>
+      </c>
+      <c r="D28" t="s">
+        <v>3497</v>
+      </c>
+      <c r="E28" t="s">
+        <v>670</v>
+      </c>
+      <c r="F28" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>3508</v>
+      </c>
+      <c r="B29" t="s">
+        <v>3509</v>
+      </c>
+      <c r="C29" t="s">
+        <v>3511</v>
+      </c>
+      <c r="D29" t="s">
+        <v>3498</v>
+      </c>
+      <c r="E29" t="s">
+        <v>2517</v>
+      </c>
+      <c r="F29" t="s">
+        <v>2518</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>3508</v>
+      </c>
+      <c r="B30" t="s">
+        <v>3509</v>
+      </c>
+      <c r="C30" t="s">
+        <v>221</v>
+      </c>
+      <c r="D30" t="s">
+        <v>3495</v>
+      </c>
+      <c r="E30">
+        <v>65</v>
+      </c>
+      <c r="F30" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>3508</v>
+      </c>
+      <c r="B31" t="s">
+        <v>3509</v>
+      </c>
+      <c r="C31" t="s">
+        <v>221</v>
+      </c>
+      <c r="D31" t="s">
+        <v>3496</v>
+      </c>
+      <c r="E31">
+        <v>132</v>
+      </c>
+      <c r="F31" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>3508</v>
+      </c>
+      <c r="B32" t="s">
+        <v>3509</v>
+      </c>
+      <c r="C32" t="s">
+        <v>221</v>
+      </c>
+      <c r="D32" t="s">
+        <v>3497</v>
+      </c>
+      <c r="E32" t="s">
+        <v>1180</v>
+      </c>
+      <c r="F32" t="s">
+        <v>1181</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C81"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -12176,7 +14079,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
           <x14:formula1>
             <xm:f>Helper!$A$2:$A$15</xm:f>
           </x14:formula1>
@@ -12188,11 +14091,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D365"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
@@ -15356,7 +17259,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000000000000}">
           <x14:formula1>
             <xm:f>Helper!$A$2:$A$15</xm:f>
           </x14:formula1>
@@ -15368,8 +17271,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F602"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -21027,9 +22930,6 @@
       <c r="B345" t="s">
         <v>204</v>
       </c>
-      <c r="C345" t="s">
-        <v>86</v>
-      </c>
       <c r="E345" t="str">
         <f>INDEX(coco_classes!C:C,MATCH(LOWER(OpenImages_classes!B345),coco_classes!B:B,0))</f>
         <v>Device Indicators</v>
@@ -25224,12 +27124,12 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F602"/>
+  <autoFilter ref="A1:F602" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0300-000000000000}">
           <x14:formula1>
             <xm:f>Helper!$A$2:$A$15</xm:f>
           </x14:formula1>
@@ -25241,11 +27141,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A524" workbookViewId="0">
+    <sheetView topLeftCell="A524" workbookViewId="0">
       <selection activeCell="B563" sqref="B563"/>
     </sheetView>
   </sheetViews>
@@ -37256,9 +39156,6 @@
       <c r="B600" t="s">
         <v>2697</v>
       </c>
-      <c r="C600" t="s">
-        <v>86</v>
-      </c>
       <c r="E600" t="e">
         <f>INDEX(coco_classes!C:C,MATCH(LOWER(ImageNet_classes!B600),coco_classes!B:B,0))</f>
         <v>#N/A</v>
@@ -45446,12 +47343,12 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G1001"/>
+  <autoFilter ref="A1:G1001" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0400-000000000000}">
           <x14:formula1>
             <xm:f>Helper!$A$2:$A$15</xm:f>
           </x14:formula1>

</xml_diff>